<commit_message>
-e and -m options was added
</commit_message>
<xml_diff>
--- a/data/formats.xlsx
+++ b/data/formats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
   <si>
     <t>3gp</t>
   </si>
@@ -439,7 +439,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,6 +468,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
@@ -479,6 +482,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
       <c r="D3">
         <v>0</v>
       </c>
@@ -546,6 +552,9 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
       <c r="D8">
         <v>0</v>
       </c>
@@ -557,6 +566,9 @@
       <c r="B9" t="s">
         <v>9</v>
       </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
       <c r="D9">
         <v>0</v>
       </c>
@@ -1123,6 +1135,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>